<commit_message>
correcting liberty grade on T test
</commit_message>
<xml_diff>
--- a/Teste T.xlsx
+++ b/Teste T.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I852573\Documents\Colling\Facul\Simulação\online-tickets-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3594C804-7142-4A76-A0BF-EB407A65C2F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD682D22-9202-4082-A277-A4F73D364FEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
   <si>
     <t>Teste-t: duas amostras presumindo variâncias equivalentes</t>
   </si>
@@ -66,18 +66,6 @@
   </si>
   <si>
     <t>Stat t</t>
-  </si>
-  <si>
-    <t>P(T&lt;=t) uni-caudal</t>
-  </si>
-  <si>
-    <t>t crítico uni-caudal</t>
-  </si>
-  <si>
-    <t>P(T&lt;=t) bi-caudal</t>
-  </si>
-  <si>
-    <t>t crítico bi-caudal</t>
   </si>
   <si>
     <r>
@@ -115,65 +103,20 @@
     <t>t=</t>
   </si>
   <si>
+    <t>médias</t>
+  </si>
+  <si>
+    <t>desvios</t>
+  </si>
+  <si>
+    <t>Sist - Mod</t>
+  </si>
+  <si>
+    <t>n=</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">procura </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>/2</t>
-    </r>
-  </si>
-  <si>
-    <t>médias</t>
-  </si>
-  <si>
-    <t>desvios</t>
-  </si>
-  <si>
-    <t>Sist - Mod</t>
-  </si>
-  <si>
-    <t>n=</t>
-  </si>
-  <si>
-    <r>
-      <t>Com t = -0,12034  &lt;  tval (2.306)  logo não rejeita H</t>
+      <t>Com t = -0,12034  &lt;  tval (2,179)  logo não rejeita H</t>
     </r>
     <r>
       <rPr>
@@ -193,7 +136,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,13 +192,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Symbol"/>
-      <family val="1"/>
-      <charset val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -336,8 +272,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -345,9 +283,7 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -357,22 +293,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -381,15 +315,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,170 +339,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>190127</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1847849" y="2380877"/>
-          <a:ext cx="4124326" cy="2600697"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagem 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6076950" y="3114675"/>
-          <a:ext cx="2781300" cy="1524000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1771650</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Elipse 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315200" y="4352925"/>
-          <a:ext cx="552450" cy="142876"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="15875">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -877,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="L16" sqref="L16:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,23 +662,23 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="10">
         <v>838</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>729</v>
       </c>
       <c r="K2" t="s">
@@ -916,27 +686,27 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+      <c r="A3" s="10">
         <v>799</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>889</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H3">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="10">
         <v>835</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>784</v>
       </c>
       <c r="D4">
@@ -947,19 +717,19 @@
         <f>7*7*(7+7-2)</f>
         <v>588</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>15</v>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="10">
         <v>812</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>853</v>
       </c>
       <c r="D5">
@@ -973,39 +743,39 @@
       <c r="K5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="15">
         <f>A12</f>
         <v>817.71428571428567</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="15">
         <f>B12</f>
         <v>820.71428571428567</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="10">
         <v>801</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>900</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="14">
         <f>A13</f>
         <v>383.90476190476193</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="14">
         <f>B13</f>
         <v>6141.9047619047624</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="10">
         <v>798</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>878</v>
       </c>
       <c r="D7">
@@ -1017,9 +787,9 @@
         <v>6.4807406984078604</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="6">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5">
         <f>D7*F7</f>
         <v>-0.12033686900046135</v>
       </c>
@@ -1034,10 +804,10 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="10">
         <v>841</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <v>712</v>
       </c>
       <c r="K8" s="3" t="s">
@@ -1049,13 +819,13 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
       <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="21">
-        <v>2306</v>
+        <v>9</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2.1789999999999998</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>5</v>
@@ -1066,70 +836,55 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="11"/>
-      <c r="K10" s="3" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="K10" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="3">
-        <v>8</v>
-      </c>
-      <c r="M10" s="3"/>
+      <c r="L10">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
-      <c r="B11" s="11"/>
-      <c r="D11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="3" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="9"/>
+      <c r="D11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="19">
         <f>H7</f>
         <v>-0.12033686900046135</v>
       </c>
-      <c r="M11" s="3"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <f>AVERAGE(A2:A8)</f>
         <v>817.71428571428567</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <f>AVERAGE(B2:B8)</f>
         <v>820.71428571428567</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L12" s="3">
-        <v>0.17183499138931238</v>
-      </c>
-      <c r="M12" s="3"/>
+      <c r="C12" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <f>_xlfn.VAR.S(A2:A8)</f>
         <v>383.90476190476193</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <f>_xlfn.VAR.S(B2:B8)</f>
         <v>6141.9047619047624</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="3">
-        <v>1.8595480375308981</v>
-      </c>
-      <c r="M13" s="3"/>
+      <c r="C13" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1140,48 +895,26 @@
         <f>SQRT(B13)</f>
         <v>78.370305357991057</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="3">
-        <v>0.34366998277862476</v>
-      </c>
-      <c r="M14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="K15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="15">
-        <v>2.3060041352041671</v>
-      </c>
-      <c r="M15" s="4"/>
+      <c r="C14" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="L17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="N17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>